<commit_message>
fixed grousize for phq/hads
</commit_message>
<xml_diff>
--- a/01_data/SUBSET_HADS.xlsx
+++ b/01_data/SUBSET_HADS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t xml:space="preserve">Study</t>
   </si>
@@ -254,58 +254,130 @@
     <t xml:space="preserve">Sundquist J., Lilja A., Palmer K., Memon A.A., Wang X., Johansson L.M., und Sundquist K. „Mindfulness group therapy in primary care patients with depression, anxiety and stress and adjustment disorders: Randomised controlled trial“. British Journal of Psychiatry 206, Nr. 2 (2015): 128–35. https://doi.org/10.1192/bjp.bp.114.150243.</t>
   </si>
   <si>
+    <t xml:space="preserve">110</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sajobi T.T., Jette N., Fiest K.M., Patten S.B., Engbers J.D.T., Lowerison M.W., und Wiebe S. „Correlates of disability related to seizures in persons with epilepsy“. Epilepsia 56, Nr. 9 (2015): 1463–69. https://doi.org/10.1111/epi.13102.</t>
   </si>
   <si>
+    <t xml:space="preserve">241</t>
+  </si>
+  <si>
     <t xml:space="preserve">Weber T., Eberle J., Messelhauser U., Schiffmann L., Nies C., Schabram J., Zielke A., u. a. „Parathyroidectomy, elevated depression scores, and suicidal ideation in patients with primary hyperparathyroidism: Results of a prospective multicenter study“. JAMA Surgery 148, Nr. 2 (2013): 109–15. https://doi.org/10.1001/2013.jamasurg.316.</t>
   </si>
   <si>
+    <t xml:space="preserve">194</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fischer H.F., Klug C., Roeper K., Blozik E., Edelmann F., Eisele M., Stork S., u. a. „Screening for mental disorders in heart failure patients using computer-adaptive tests“. Quality of life research : an international journal of quality of life aspects of treatment, care and rehabilitation 23, Nr. 5 (2014): 1609–18. n.</t>
   </si>
   <si>
     <t xml:space="preserve">Hoerger M., Greer J.A., Jackson V.A., Park E.R., Pirl W.F., El-Jawahri A., Gallagher E.R., u. a. „Defining the elements of early palliative care that are associated with patient-reported outcomes and the delivery of end-of-life care“. Journal of Clinical Oncology 36, Nr. 11 (2018): 1096–1102. https://doi.org/10.1200/JCO.2017.75.6676.</t>
   </si>
   <si>
+    <t xml:space="preserve">171</t>
+  </si>
+  <si>
     <t xml:space="preserve">Geraghty A.W.A., Stuart B., Terluin B., Kendrick T., Little P., und Moore M. „Distinguishing between emotional distress and psychiatric disorder in primary care attenders: A cross sectional study of the four-dimensional symptom questionnaire (4DSQ)“. Journal of Affective Disorders 184, Nr. (Geraghty, Stuart, Kendrick, Little, Moore) Primary Care and Population Sciences, Aldermoor Health Centre, University of Southampton, Aldermoor Close, Southampton, Hampshire SO16 5ST, United Kingdom (2015): 198–204. https://doi.org/10.1016/j.jad.2015.05.064.</t>
   </si>
   <si>
+    <t xml:space="preserve">487</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chung J., Ju G., Yang J., Jeong J., Jeong Y., Choi M.K., Kwon J., Lee K.H., Kim S.T., und Han H.S. „Prevalence of and factors associated with anxiety and depression in Korean patients with newly diagnosed advanced gastrointestinal cancer“. Korean Journal of Internal Medicine 33, Nr. 3 (2018): 585–94. https://doi.org/10.3904/kjim.2016.108.</t>
   </si>
   <si>
+    <t xml:space="preserve">71</t>
+  </si>
+  <si>
     <t xml:space="preserve">De Fazio P., Cerminara G., Ruberto S., Caroleo M., Puca M., Rania O., Suffredini E., Procopio L., und Segura-Garcia C. „Hospitalization and other risk factors for depressive and anxious symptoms in oncological and non-oncological patients“. Psycho-Oncology 26, Nr. 4 (2017): 493–99. https://doi.org/10.1002/pon.4170.</t>
   </si>
   <si>
+    <t xml:space="preserve">154</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chung S., Kang S.-H., Kweon K., Youn S., Kang H.S., Hong S.-B., und Hong S.-J. „Cognitive emotion regulation strategies and insomnia or other psychiatric Symptoms among humidifier disinfectant victims“. Sleep Medicine Research 9, Nr. 1 (2018): 26–31. https://doi.org/10.17241/smr.2018.00136.</t>
   </si>
   <si>
     <t xml:space="preserve">Turner A., Hambridge J., White J., Carter G., Clover K., Nelson L., und Hackett M. „Depression screening in stroke: A comparison of alternative measures with the structured diagnostic interview for the diagnostic and statistical manual of mental disorders, fourth edition (major depressive episode) as criterion standard“. Stroke 43, Nr. 4 (2012): 1000–1005. https://doi.org/10.1161/STROKEAHA.111.643296.</t>
   </si>
   <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hansson M., Chotai J., Nordstom A., und Bodlund O. „Comparison of two self-rating scales to detect depression: HADS and PHQ-9“. British Journal of General Practice 59, Nr. 566 (2009): 650–54. https://doi.org/10.3399/bjgp09X454070.</t>
   </si>
   <si>
+    <t xml:space="preserve">737</t>
+  </si>
+  <si>
     <t xml:space="preserve">Okuda T., Asano K., Numata N., Hirano Y., Yamamoto T., Tanaka M., Matsuzawa D., Shimizu E., Iyo M., und Nakazato M. „Feasibility of cognitive remediation therapy for adults with autism spectrum disorders: A single-group pilot study“. Neuropsychiatric Disease and Treatment 13, Nr. (Okuda, Asano, Hirano, Shimizu, Nakazato) Division of Cognitive Behavioral Science, United Graduate School of Child Development, Osaka University, Kanazawa University, Hamamatsu University School of Medicine, Chiba University and University of Fukui, Chiba-shi, Chiba, Japan (2017): 2185–91. https://doi.org/10.2147/NDT.S141555.</t>
   </si>
   <si>
     <t xml:space="preserve">Nanni M.G., Caruso R., Travado L., Ventura C., Palma A., Berardi A.M., Meggiolaro E., u. a. „Relationship of demoralization with anxiety, depression, and quality of life: A Southern European study of Italian and Portuguese cancer patients“. Psycho-Oncology 27, Nr. 11 (2018): 2616–22. https://doi.org/10.1002/pon.4824.</t>
   </si>
   <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
     <t xml:space="preserve">Haddad M., Walters P., Phillips R., Tsakok J., Williams P., Mann A., und Tylee A. „Detecting Depression in Patients with Coronary Heart Disease: A Diagnostic Evaluation of the PHQ-9 and HADS-D in Primary Care, Findings From the UPBEAT-UK Study“. PLoS ONE 8, Nr. 10 (2013): e78493. https://doi.org/10.1371/journal.pone.0078493.</t>
   </si>
   <si>
+    <t xml:space="preserve">698</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ma H., Wang Y., Xue Y., Huang D., Kong Y., Zhao X., und Zhang M. „The effect of Xinkeshu tablets on depression and anxiety symptoms in patients with coronary artery disease: Results from a double-blind, randomized, placebo-controlled study“. Biomedicine and Pharmacotherapy 112, Nr. (Ma, Wang) Guangdong Cardiovascular Institute, Guangdong Provincial People’s Hospital, Guangdong Academy of Medical Sciences, Guangdong, China (2019): 108639. https://doi.org/10.1016/j.biopha.2019.108639.</t>
   </si>
   <si>
     <t xml:space="preserve">———. „Psychometric comparison of PHQ-9 and HADS for measuring depression severity in primary care“. British Journal of General Practice 58, Nr. 546 (2008): 32–36. https://doi.org/10.3399/bjgp08X263794.</t>
   </si>
   <si>
+    <t xml:space="preserve">544</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sajobi T.T., Amoozegar F., Wang M., Wiebe N., Fiest K.M., Patten S.B., und Jette N. „Global assessment of migraine severity measure: Preliminary evidence of construct validity“. BMC Neurology 19, Nr. 1 (2019): 53. https://doi.org/10.1186/s12883-019-1284-8.</t>
   </si>
   <si>
+    <t xml:space="preserve">263</t>
+  </si>
+  <si>
     <t xml:space="preserve">Schaeffeler N., Pfeiffer K., Ringwald J., Brucker S., Wallwiener M., Zipfel S., und Teufel M. „Assessing the need for psychooncological support: Screening instruments in combination with patients’ subjective evaluation may define psychooncological pathways“. Psycho-Oncology 24, Nr. 12 (2015): 1784–91. https://doi.org/10.1002/pon.3855.</t>
   </si>
   <si>
+    <t xml:space="preserve">135</t>
+  </si>
+  <si>
     <t xml:space="preserve">Haussmann A., Schaffeler N., Hautzinger M., Weyel B., Eigentler T., Zipfel S., und Teufel M. „Religious/Spiritual Needs and Psychosocial Burden of Melanoma Patients“. PPmP Psychotherapie Psychosomatik Medizinische Psychologie, Religiose/spirituelle Bedurfnisse und psychosoziale Belastung von Patienten mit malignem Melanom, 67, Nr. 9–10 (2017): 413–19. https://doi.org/10.1055/s-0043-101373.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nicht berichtet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
   </si>
   <si>
     <t xml:space="preserve">3#2 timepoint</t>
@@ -2020,11 +2092,13 @@
       <c r="E69" t="s">
         <v>8</v>
       </c>
-      <c r="F69"/>
+      <c r="F69" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -2038,11 +2112,13 @@
       <c r="E70" t="s">
         <v>8</v>
       </c>
-      <c r="F70"/>
+      <c r="F70" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -2056,11 +2132,13 @@
       <c r="E71" t="s">
         <v>8</v>
       </c>
-      <c r="F71"/>
+      <c r="F71" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -2074,11 +2152,13 @@
       <c r="E72" t="s">
         <v>8</v>
       </c>
-      <c r="F72"/>
+      <c r="F72" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -2092,11 +2172,13 @@
       <c r="E73" t="s">
         <v>8</v>
       </c>
-      <c r="F73"/>
+      <c r="F73" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -2110,11 +2192,13 @@
       <c r="E74" t="s">
         <v>8</v>
       </c>
-      <c r="F74"/>
+      <c r="F74" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -2128,11 +2212,13 @@
       <c r="E75" t="s">
         <v>8</v>
       </c>
-      <c r="F75"/>
+      <c r="F75" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -2146,11 +2232,13 @@
       <c r="E76" t="s">
         <v>8</v>
       </c>
-      <c r="F76"/>
+      <c r="F76" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -2164,11 +2252,13 @@
       <c r="E77" t="s">
         <v>8</v>
       </c>
-      <c r="F77"/>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -2182,11 +2272,13 @@
       <c r="E78" t="s">
         <v>8</v>
       </c>
-      <c r="F78"/>
+      <c r="F78" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2200,11 +2292,13 @@
       <c r="E79" t="s">
         <v>8</v>
       </c>
-      <c r="F79"/>
+      <c r="F79" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2218,11 +2312,13 @@
       <c r="E80" t="s">
         <v>8</v>
       </c>
-      <c r="F80"/>
+      <c r="F80" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2236,11 +2332,13 @@
       <c r="E81" t="s">
         <v>8</v>
       </c>
-      <c r="F81"/>
+      <c r="F81" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -2254,11 +2352,13 @@
       <c r="E82" t="s">
         <v>8</v>
       </c>
-      <c r="F82"/>
+      <c r="F82" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
@@ -2272,11 +2372,13 @@
       <c r="E83" t="s">
         <v>8</v>
       </c>
-      <c r="F83"/>
+      <c r="F83" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -2290,11 +2392,13 @@
       <c r="E84" t="s">
         <v>8</v>
       </c>
-      <c r="F84"/>
+      <c r="F84" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -2308,11 +2412,13 @@
       <c r="E85" t="s">
         <v>8</v>
       </c>
-      <c r="F85"/>
+      <c r="F85" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
@@ -2326,11 +2432,13 @@
       <c r="E86" t="s">
         <v>8</v>
       </c>
-      <c r="F86"/>
+      <c r="F86" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
@@ -2344,7 +2452,9 @@
       <c r="E87" t="s">
         <v>8</v>
       </c>
-      <c r="F87"/>
+      <c r="F87" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
@@ -2362,11 +2472,13 @@
       <c r="E88" t="s">
         <v>27</v>
       </c>
-      <c r="F88"/>
+      <c r="F88" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
         <v>26</v>
@@ -2380,11 +2492,13 @@
       <c r="E89" t="s">
         <v>27</v>
       </c>
-      <c r="F89"/>
+      <c r="F89" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B90" t="s">
         <v>26</v>
@@ -2398,11 +2512,13 @@
       <c r="E90" t="s">
         <v>27</v>
       </c>
-      <c r="F90"/>
+      <c r="F90" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
         <v>26</v>
@@ -2416,11 +2532,13 @@
       <c r="E91" t="s">
         <v>27</v>
       </c>
-      <c r="F91"/>
+      <c r="F91" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B92" t="s">
         <v>26</v>
@@ -2434,11 +2552,13 @@
       <c r="E92" t="s">
         <v>27</v>
       </c>
-      <c r="F92"/>
+      <c r="F92" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
         <v>26</v>
@@ -2452,11 +2572,13 @@
       <c r="E93" t="s">
         <v>27</v>
       </c>
-      <c r="F93"/>
+      <c r="F93" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B94" t="s">
         <v>26</v>
@@ -2470,11 +2592,13 @@
       <c r="E94" t="s">
         <v>27</v>
       </c>
-      <c r="F94"/>
+      <c r="F94" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B95" t="s">
         <v>26</v>
@@ -2488,11 +2612,13 @@
       <c r="E95" t="s">
         <v>27</v>
       </c>
-      <c r="F95"/>
+      <c r="F95" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
         <v>26</v>
@@ -2506,11 +2632,13 @@
       <c r="E96" t="s">
         <v>27</v>
       </c>
-      <c r="F96"/>
+      <c r="F96" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B97" t="s">
         <v>30</v>
@@ -2524,11 +2652,13 @@
       <c r="E97" t="s">
         <v>27</v>
       </c>
-      <c r="F97"/>
+      <c r="F97" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B98" t="s">
         <v>33</v>
@@ -2542,11 +2672,13 @@
       <c r="E98" t="s">
         <v>8</v>
       </c>
-      <c r="F98"/>
+      <c r="F98" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B99" t="s">
         <v>33</v>
@@ -2560,11 +2692,13 @@
       <c r="E99" t="s">
         <v>8</v>
       </c>
-      <c r="F99"/>
+      <c r="F99" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>33</v>
@@ -2578,11 +2712,13 @@
       <c r="E100" t="s">
         <v>8</v>
       </c>
-      <c r="F100"/>
+      <c r="F100" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B101" t="s">
         <v>33</v>
@@ -2596,11 +2732,13 @@
       <c r="E101" t="s">
         <v>8</v>
       </c>
-      <c r="F101"/>
+      <c r="F101" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B102" t="s">
         <v>35</v>
@@ -2614,11 +2752,13 @@
       <c r="E102" t="s">
         <v>27</v>
       </c>
-      <c r="F102"/>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B103" t="s">
         <v>35</v>
@@ -2632,14 +2772,16 @@
       <c r="E103" t="s">
         <v>27</v>
       </c>
-      <c r="F103"/>
+      <c r="F103" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="C104" t="n">
         <v>7.14</v>
@@ -2648,13 +2790,15 @@
         <v>55.4242606320608</v>
       </c>
       <c r="E104" t="s">
-        <v>99</v>
-      </c>
-      <c r="F104"/>
+        <v>123</v>
+      </c>
+      <c r="F104" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B105" t="s">
         <v>36</v>
@@ -2668,11 +2812,13 @@
       <c r="E105" t="s">
         <v>8</v>
       </c>
-      <c r="F105"/>
+      <c r="F105" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B106" t="s">
         <v>36</v>
@@ -2686,11 +2832,13 @@
       <c r="E106" t="s">
         <v>8</v>
       </c>
-      <c r="F106"/>
+      <c r="F106" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B107" t="s">
         <v>77</v>
@@ -2708,7 +2856,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B108" t="s">
         <v>7</v>
@@ -2722,7 +2870,9 @@
       <c r="E108" t="s">
         <v>8</v>
       </c>
-      <c r="F108"/>
+      <c r="F108" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>